<commit_message>
refactor: Letter, User의 create_at 추가
</commit_message>
<xml_diff>
--- a/docs/newYearProject_api_0.8v.xlsx
+++ b/docs/newYearProject_api_0.8v.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sujinworkspace\hello-new-year\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA9F7A4-52C2-4CD2-A9B7-1851D8C1A388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F8F2FE-A5EE-4959-A2F6-8DC4527A1029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="610" yWindow="1900" windowWidth="19420" windowHeight="15470" xr2:uid="{B39A122C-5FE9-4637-9C81-A77D518F6D51}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="61">
   <si>
     <t>HTTP</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -376,15 +376,46 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>편지 조회, 페이징적용</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>api/letter/{uuid}/getLetter</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>편지 목록 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+"resultCode": "SUCCESS",
+"result":{
+{
+"nickName":"sujan",
+"wish":"다이어트",
+"money":10000
+}
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+"resultCode": "SUCCESS",
+	"result":{
+		"author": "수진이",
+		"content": "안녕? 새해복마니바다",
+		"money": 10000
+	}
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>편지 상세 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>편지 전체 조회, 페이징적용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>api/letter/{uuid}/getLetter/{id}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -808,10 +839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D9E06A-517D-4A3E-9023-DAF9C9FD353C}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -961,10 +992,24 @@
         <v>21</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>56</v>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -976,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDE62AAF-3A38-4305-8F5C-D173E5501EE9}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1143,7 +1188,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="119" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" ht="153" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1151,7 +1196,7 @@
         <v>200</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
         <v>32</v>
@@ -1238,7 +1283,21 @@
         <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="136" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <v>200</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>